<commit_message>
Fitur Add Pelanggan dan Import Excel Done
</commit_message>
<xml_diff>
--- a/assets/export/Excel_DataPelanggan.xlsx
+++ b/assets/export/Excel_DataPelanggan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\xampp\htdocs\nakasy\assets\export\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C63E23EC-9233-47E2-9878-730D5985B906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A30153-1FAB-44F6-933D-A7FF0E133726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,9 +85,6 @@
     <t>Home 5</t>
   </si>
   <si>
-    <t>inflyajalah</t>
-  </si>
-  <si>
     <t>*12</t>
   </si>
   <si>
@@ -110,6 +107,9 @@
   </si>
   <si>
     <t>Alihadi</t>
+  </si>
+  <si>
+    <t>infly</t>
   </si>
 </sst>
 </file>
@@ -117,7 +117,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -260,7 +260,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -605,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -637,10 +637,10 @@
       <c r="E1" s="12"/>
       <c r="F1" s="12"/>
       <c r="G1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>25</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>26</v>
       </c>
       <c r="I1" s="13"/>
       <c r="J1" s="13"/>
@@ -660,7 +660,7 @@
       <c r="F2" s="12"/>
       <c r="G2" s="9"/>
       <c r="H2" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I2" s="13"/>
       <c r="J2" s="13"/>
@@ -765,25 +765,25 @@
         <v>19</v>
       </c>
       <c r="G6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="J6" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>24</v>
       </c>
       <c r="K6" s="11">
         <v>44208</v>
       </c>
       <c r="M6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N6" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>